<commit_message>
Updated POs and added more functions
</commit_message>
<xml_diff>
--- a/src/main/resources/excels/PlanPermission.xlsx
+++ b/src/main/resources/excels/PlanPermission.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\IdeaProjects\GoSELL-Automation\src\main\resources\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\GoSELL-Automation\src\main\resources\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A7C99F-DFF8-433E-927B-37DCC25793A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EFC003-4A5B-4879-8A0A-846AB21480F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="4116" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13220" windowHeight="4120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="124">
   <si>
     <t>MenuItem</t>
   </si>
@@ -211,9 +211,6 @@
     <t>/call-center/intro</t>
   </si>
   <si>
-    <t>Call History</t>
-  </si>
-  <si>
     <t>Cashbook</t>
   </si>
   <si>
@@ -386,13 +383,22 @@
   </si>
   <si>
     <t>/setting</t>
+  </si>
+  <si>
+    <t>GoFree</t>
+  </si>
+  <si>
+    <t>Greyed Out</t>
+  </si>
+  <si>
+    <t>Call Center-Call History</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -448,6 +454,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -506,7 +520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -528,6 +542,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,18 +764,18 @@
   <dimension ref="A1:AB62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" customWidth="1"/>
-    <col min="2" max="2" width="37.77734375" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="26.81640625" customWidth="1"/>
+    <col min="2" max="2" width="37.81640625" customWidth="1"/>
+    <col min="3" max="3" width="22.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -785,8 +800,11 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -811,7 +829,9 @@
       <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -832,7 +852,7 @@
       <c r="AA2" s="3"/>
       <c r="AB2" s="3"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -857,7 +877,9 @@
       <c r="H3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -878,7 +900,7 @@
       <c r="AA3" s="3"/>
       <c r="AB3" s="3"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -903,8 +925,11 @@
       <c r="H4" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -929,8 +954,11 @@
       <c r="H5" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -955,7 +983,9 @@
       <c r="H6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -976,7 +1006,7 @@
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1001,8 +1031,11 @@
       <c r="H7" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I7" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -1027,8 +1060,11 @@
       <c r="H8" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I8" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
@@ -1053,8 +1089,11 @@
       <c r="H9" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I9" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>26</v>
       </c>
@@ -1079,8 +1118,11 @@
       <c r="H10" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I10" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
@@ -1105,8 +1147,11 @@
       <c r="H11" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I11" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>30</v>
       </c>
@@ -1131,8 +1176,11 @@
       <c r="H12" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I12" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
@@ -1157,8 +1205,11 @@
       <c r="H13" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I13" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
@@ -1183,7 +1234,9 @@
       <c r="H14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="3"/>
+      <c r="I14" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -1204,7 +1257,7 @@
       <c r="AA14" s="3"/>
       <c r="AB14" s="3"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>36</v>
       </c>
@@ -1229,8 +1282,11 @@
       <c r="H15" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I15" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>37</v>
       </c>
@@ -1255,8 +1311,11 @@
       <c r="H16" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I16" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>39</v>
       </c>
@@ -1281,8 +1340,11 @@
       <c r="H17" s="20" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I17" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>41</v>
       </c>
@@ -1307,8 +1369,11 @@
       <c r="H18" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I18" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>42</v>
       </c>
@@ -1333,8 +1398,11 @@
       <c r="H19" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I19" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>44</v>
       </c>
@@ -1359,8 +1427,11 @@
       <c r="H20" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I20" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>46</v>
       </c>
@@ -1385,8 +1456,11 @@
       <c r="H21" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I21" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>48</v>
       </c>
@@ -1411,7 +1485,9 @@
       <c r="H22" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I22" s="3"/>
+      <c r="I22" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
@@ -1432,7 +1508,7 @@
       <c r="AA22" s="3"/>
       <c r="AB22" s="3"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>50</v>
       </c>
@@ -1457,7 +1533,9 @@
       <c r="H23" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="I23" s="3"/>
+      <c r="I23" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
@@ -1478,7 +1556,7 @@
       <c r="AA23" s="3"/>
       <c r="AB23" s="3"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>52</v>
       </c>
@@ -1503,8 +1581,11 @@
       <c r="H24" s="18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I24" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>53</v>
       </c>
@@ -1529,8 +1610,11 @@
       <c r="H25" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I25" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>55</v>
       </c>
@@ -1555,7 +1639,9 @@
       <c r="H26" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I26" s="3"/>
+      <c r="I26" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
@@ -1576,7 +1662,7 @@
       <c r="AA26" s="3"/>
       <c r="AB26" s="3"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
@@ -1601,8 +1687,11 @@
       <c r="H27" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I27" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>59</v>
       </c>
@@ -1627,8 +1716,11 @@
       <c r="H28" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I28" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>61</v>
       </c>
@@ -1653,7 +1745,9 @@
       <c r="H29" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I29" s="3"/>
+      <c r="I29" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
@@ -1674,9 +1768,9 @@
       <c r="AA29" s="3"/>
       <c r="AB29" s="3"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>63</v>
+        <v>123</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>62</v>
@@ -1699,7 +1793,9 @@
       <c r="H30" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I30" s="9"/>
+      <c r="I30" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
@@ -1720,13 +1816,13 @@
       <c r="AA30" s="9"/>
       <c r="AB30" s="9"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C31" s="2" t="s">
         <v>10</v>
       </c>
@@ -1745,7 +1841,9 @@
       <c r="H31" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I31" s="3"/>
+      <c r="I31" s="21" t="s">
+        <v>122</v>
+      </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
@@ -1766,12 +1864,12 @@
       <c r="AA31" s="3"/>
       <c r="AB31" s="3"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>14</v>
@@ -1791,7 +1889,9 @@
       <c r="H32" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I32" s="3"/>
+      <c r="I32" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
@@ -1812,12 +1912,12 @@
       <c r="AA32" s="3"/>
       <c r="AB32" s="3"/>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>14</v>
@@ -1837,13 +1937,16 @@
       <c r="H33" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I33" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>14</v>
@@ -1863,14 +1966,17 @@
       <c r="H34" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I34" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="C35" s="2" t="s">
         <v>10</v>
       </c>
@@ -1889,7 +1995,9 @@
       <c r="H35" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="I35" s="3"/>
+      <c r="I35" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
@@ -1910,38 +2018,41 @@
       <c r="AA35" s="3"/>
       <c r="AB35" s="3"/>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="C36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>14</v>
@@ -1961,65 +2072,74 @@
       <c r="H37" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I37" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="C38" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="C39" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>14</v>
@@ -2039,13 +2159,16 @@
       <c r="H40" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I40" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>14</v>
@@ -2065,65 +2188,74 @@
       <c r="H41" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I41" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="C42" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+      <c r="A43" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C42" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
+      <c r="B43" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="C43" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C43" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+      <c r="B44" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>14</v>
@@ -2143,66 +2275,75 @@
       <c r="H44" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I44" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="C45" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C45" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F45" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G45" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H45" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="C46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G46" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H46" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="C47" s="2" t="s">
         <v>10</v>
       </c>
@@ -2221,7 +2362,9 @@
       <c r="H47" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="I47" s="3"/>
+      <c r="I47" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
@@ -2242,38 +2385,41 @@
       <c r="AA47" s="3"/>
       <c r="AB47" s="3"/>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F48" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="G48" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H48" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+      <c r="B49" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>14</v>
@@ -2293,13 +2439,16 @@
       <c r="H49" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I49" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>14</v>
@@ -2319,13 +2468,16 @@
       <c r="H50" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I50" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>14</v>
@@ -2345,13 +2497,16 @@
       <c r="H51" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I51" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B52" s="13" t="s">
         <v>105</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>106</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>14</v>
@@ -2371,196 +2526,220 @@
       <c r="H52" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="I52" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B53" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B53" s="13" t="s">
+      <c r="C53" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+      <c r="A54" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G53" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H53" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A54" s="14" t="s">
+      <c r="B54" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="C54" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G54" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C54" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D54" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E54" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F54" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G54" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H54" s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+      <c r="B55" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B55" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G55" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H55" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
+      <c r="B56" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H56" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+      <c r="B57" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+      <c r="B58" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+      <c r="B59" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28" ht="13" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B59" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G59" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H59" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="C60" s="16" t="s">
         <v>10</v>
       </c>
@@ -2579,7 +2758,9 @@
       <c r="H60" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I60" s="3"/>
+      <c r="I60" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
@@ -2600,13 +2781,13 @@
       <c r="AA60" s="3"/>
       <c r="AB60" s="3"/>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="C61" s="16" t="s">
         <v>10</v>
       </c>
@@ -2625,7 +2806,9 @@
       <c r="H61" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I61" s="3"/>
+      <c r="I61" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
@@ -2646,13 +2829,13 @@
       <c r="AA61" s="3"/>
       <c r="AB61" s="3"/>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" ht="13" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>121</v>
-      </c>
       <c r="C62" s="16" t="s">
         <v>10</v>
       </c>
@@ -2671,7 +2854,9 @@
       <c r="H62" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I62" s="3"/>
+      <c r="I62" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>

</xml_diff>